<commit_message>
added some templates and dropdown
</commit_message>
<xml_diff>
--- a/Events_Data.xlsx
+++ b/Events_Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t xml:space="preserve">EVENT ID</t>
   </si>
@@ -37,6 +37,15 @@
     <t xml:space="preserve">NUMBER OF ROUNDS</t>
   </si>
   <si>
+    <t xml:space="preserve">GENDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CATEGORY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB CATEGORY</t>
+  </si>
+  <si>
     <t xml:space="preserve">COST</t>
   </si>
   <si>
@@ -49,6 +58,15 @@
     <t xml:space="preserve">Networking Event</t>
   </si>
   <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cat1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub1</t>
+  </si>
+  <si>
     <t xml:space="preserve">International Conference on Social Science and Humanities</t>
   </si>
   <si>
@@ -56,6 +74,12 @@
   </si>
   <si>
     <t xml:space="preserve">Conference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cat2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub2</t>
   </si>
 </sst>
 </file>
@@ -334,10 +358,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -346,10 +370,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="19.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="31.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="22.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="20.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="16.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="31.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -368,8 +392,17 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -377,18 +410,27 @@
         <v>12345</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -397,18 +439,27 @@
         <v>99999</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="1" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>